<commit_message>
march2021 xs and xl allocation
</commit_message>
<xml_diff>
--- a/allocation_next_month.xlsx
+++ b/allocation_next_month.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FWallace/Shopify/allocation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C024243-4BE9-2A43-A1FE-734C91B29B31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E5C1C90D-372E-EC41-A5E5-2F9EEC3E89A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2500" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="7900" yWindow="2640" windowWidth="27640" windowHeight="16940"/>
   </bookViews>
   <sheets>
     <sheet name="allocation_next_month" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>count</t>
   </si>
@@ -28,27 +28,6 @@
     <t>product_collection</t>
   </si>
   <si>
-    <t xml:space="preserve"> Guiding Light - 3 Items</t>
-  </si>
-  <si>
-    <t>Coral Kissed - 2 Items</t>
-  </si>
-  <si>
-    <t>Coral Kissed - 3 Items</t>
-  </si>
-  <si>
-    <t>Coral Kissed - 5 Items</t>
-  </si>
-  <si>
-    <t>Daily Mantra - 2 Items</t>
-  </si>
-  <si>
-    <t>Daily Mantra - 3 Items</t>
-  </si>
-  <si>
-    <t>Daily Mantra - 5 Items</t>
-  </si>
-  <si>
     <t>Ellie Picks - 2 Items</t>
   </si>
   <si>
@@ -58,115 +37,61 @@
     <t>Ellie Picks - 5 Items</t>
   </si>
   <si>
-    <t>Force Of Nature - 2 Items</t>
-  </si>
-  <si>
-    <t>Force Of Nature - 3 Items</t>
-  </si>
-  <si>
-    <t>Force Of Nature - 5 Items</t>
-  </si>
-  <si>
-    <t>Full Bloom - 5 Items</t>
+    <t>Iridescent Dreams - 2 Items</t>
+  </si>
+  <si>
+    <t>Iridescent Dreams - 3 Items</t>
+  </si>
+  <si>
+    <t>Iridescent Dreams - 5 Items</t>
+  </si>
+  <si>
+    <t>Midnight Garden - 2 Items</t>
+  </si>
+  <si>
+    <t>Midnight Garden - 3 Items</t>
+  </si>
+  <si>
+    <t>Midnight Garden - 5 Items</t>
+  </si>
+  <si>
+    <t>Punchline - 2 Items</t>
+  </si>
+  <si>
+    <t>Punchline - 3 Items</t>
+  </si>
+  <si>
+    <t>Punchline - 5 Items</t>
+  </si>
+  <si>
+    <t>Rosy Outlook - 2 Items</t>
+  </si>
+  <si>
+    <t>Rosy Outlook - 3 Items</t>
+  </si>
+  <si>
+    <t>Rosy Outlook - 5 Items</t>
+  </si>
+  <si>
+    <t>Tilt The Scale - 2 Items</t>
+  </si>
+  <si>
+    <t>Tilt The Scale - 3 Items</t>
+  </si>
+  <si>
+    <t>Tilt The Scale - 5 Items</t>
   </si>
   <si>
     <t>Funfetti - 2 Items</t>
   </si>
   <si>
-    <t>Funfetti - 3 Items</t>
-  </si>
-  <si>
-    <t>Funfetti - 5 Items</t>
-  </si>
-  <si>
-    <t>Glamazon - 3 Items</t>
-  </si>
-  <si>
-    <t>Grayscale - 2 Items</t>
-  </si>
-  <si>
-    <t>Grayscale - 3 Items</t>
-  </si>
-  <si>
-    <t>Grayscale - 5 Items</t>
-  </si>
-  <si>
-    <t>Guiding Light - 3 Items</t>
-  </si>
-  <si>
-    <t>Island Splash - 2 Items</t>
-  </si>
-  <si>
-    <t>Island Splash - 3 Items</t>
-  </si>
-  <si>
-    <t>Island Splash - 5 Items</t>
-  </si>
-  <si>
-    <t>Island Sunrise - 2 Items</t>
-  </si>
-  <si>
-    <t>Island Sunrise - 3 Items</t>
-  </si>
-  <si>
-    <t>Island Sunrise - 5 Items</t>
-  </si>
-  <si>
-    <t>Malibu Moment - 3 Items</t>
-  </si>
-  <si>
-    <t>Mauve Noir - 3 Items</t>
-  </si>
-  <si>
-    <t>Midnight Sky - 3 Items</t>
-  </si>
-  <si>
-    <t>Midnight Sky - 5 Items</t>
-  </si>
-  <si>
-    <t>On The Run - 2 Items</t>
-  </si>
-  <si>
-    <t>On The Run - 3 Items</t>
-  </si>
-  <si>
-    <t>On The Run - 5 Items</t>
-  </si>
-  <si>
-    <t>Polar Perfection - 3 Items</t>
-  </si>
-  <si>
-    <t>Polar Perfection - 5 Items</t>
-  </si>
-  <si>
-    <t>Posies In Paris - 3 Items</t>
-  </si>
-  <si>
-    <t>Posies In Paris - 5 Items</t>
-  </si>
-  <si>
-    <t>Purple Haze - 3 Items</t>
-  </si>
-  <si>
-    <t>Purple Haze - 5 Items</t>
-  </si>
-  <si>
-    <t>Wine Down - 3 Items</t>
-  </si>
-  <si>
-    <t>Winter Bloom - 3 Items</t>
-  </si>
-  <si>
-    <t>Winter Bloom - 5 Items</t>
-  </si>
-  <si>
-    <t>Fresh Tone - 3 Items</t>
-  </si>
-  <si>
-    <t>Purple Haze - 2 Items</t>
-  </si>
-  <si>
-    <t>Orders</t>
+    <t>Heart Felt - 3 Items</t>
+  </si>
+  <si>
+    <t>SUBSCRIPTIONS</t>
+  </si>
+  <si>
+    <t>ORDERS</t>
   </si>
 </sst>
 </file>
@@ -309,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,6 +412,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -650,8 +581,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1007,463 +939,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>17</v>
+        <v>1180</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>305</v>
+        <v>16260</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>142</v>
+        <v>481</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>24</v>
+        <v>1536</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1295</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>16389</v>
+        <v>777</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2984</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>140</v>
+        <v>232</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>562</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1331</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>944</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>284</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>142</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1669</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>249</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>388</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
         <v>8</v>
       </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>251</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>307</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>15</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>395</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>45</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>303</v>
-      </c>
-      <c r="B28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>52</v>
-      </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>2</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>3</v>
-      </c>
-      <c r="B31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>20</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>393</v>
-      </c>
-      <c r="B35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>59</v>
-      </c>
-      <c r="B36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>2</v>
-      </c>
-      <c r="B37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>5</v>
-      </c>
-      <c r="B39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>5</v>
-      </c>
-      <c r="B41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>2</v>
-      </c>
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>3</v>
-      </c>
-      <c r="B44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>3</v>
-      </c>
-      <c r="B48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>134</v>
-      </c>
-      <c r="B49" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>1462</v>
-      </c>
-      <c r="B50" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>385</v>
-      </c>
-      <c r="B51" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>1</v>
-      </c>
-      <c r="B52" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>6</v>
-      </c>
-      <c r="B53" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>135</v>
-      </c>
-      <c r="B54" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>29</v>
-      </c>
-      <c r="B55" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>1</v>
-      </c>
-      <c r="B56" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>11</v>
-      </c>
+      <c r="B33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>